<commit_message>
update convert to pdf using python multithread
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffa6d4cba24667ce/RPA/Personal Project/Pensie Extract Incheieri/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffa6d4cba24667ce/RPA/Personal Project/Romania-6/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{F8E41C1C-59F1-4576-A689-1D4864A3151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6DD8149-3016-4D01-9DCE-BFAA4996A543}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{F8E41C1C-59F1-4576-A689-1D4864A3151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{430E56F9-70D7-4401-BCBC-D29424989985}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Data\Input</t>
+  </si>
+  <si>
+    <t>MaxThread</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <dimension ref="A1:Z983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" activeCellId="1" sqref="C11 K11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -499,7 +502,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>